<commit_message>
Added Initial Version of Eagle CAD Workshop Files
</commit_message>
<xml_diff>
--- a/Workshop_Materials.xlsx
+++ b/Workshop_Materials.xlsx
@@ -1,26 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18229"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ALL WORKSHOP RELATED\Workshop Program Files\Workshop_Materials\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="27800" windowHeight="12590" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="120" windowWidth="27795" windowHeight="12585" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Component List" sheetId="1" r:id="rId1"/>
     <sheet name="Workshop List" sheetId="3" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="138">
   <si>
     <t>List of Components</t>
   </si>
@@ -268,18 +263,9 @@
     <t>Exercise 004: Fading While Moving</t>
   </si>
   <si>
-    <t>Arduino: Bootloader</t>
-  </si>
-  <si>
     <t>17-c</t>
   </si>
   <si>
-    <t>Practical Example: Wireless Device</t>
-  </si>
-  <si>
-    <t>4-bit Calculator (Pending)</t>
-  </si>
-  <si>
     <t>LIS3DH Sensor</t>
   </si>
   <si>
@@ -302,12 +288,153 @@
   </si>
   <si>
     <t>20-b</t>
+  </si>
+  <si>
+    <t>Component</t>
+  </si>
+  <si>
+    <t>Resistors</t>
+  </si>
+  <si>
+    <t>Switches</t>
+  </si>
+  <si>
+    <t>Buttons</t>
+  </si>
+  <si>
+    <t>Transistors/MOSFET</t>
+  </si>
+  <si>
+    <t>Relays</t>
+  </si>
+  <si>
+    <t>Diodes</t>
+  </si>
+  <si>
+    <t>OpAmp</t>
+  </si>
+  <si>
+    <t>Linear Power Regulator</t>
+  </si>
+  <si>
+    <t>Circuit</t>
+  </si>
+  <si>
+    <t>Decoupling Capacitor</t>
+  </si>
+  <si>
+    <t>Capacitors</t>
+  </si>
+  <si>
+    <t>Voltage Divider</t>
+  </si>
+  <si>
+    <t>Pull-Up Resistor</t>
+  </si>
+  <si>
+    <t>Pull-Down Resistor</t>
+  </si>
+  <si>
+    <t>Logic Level Converter</t>
+  </si>
+  <si>
+    <t>Eagle-Schem</t>
+  </si>
+  <si>
+    <t>Connectors</t>
+  </si>
+  <si>
+    <t>LED</t>
+  </si>
+  <si>
+    <t>Exercise: Simple LED Blinker</t>
+  </si>
+  <si>
+    <t>Power Regulation</t>
+  </si>
+  <si>
+    <t>Exercise: Power Output Controller</t>
+  </si>
+  <si>
+    <t>Adding Components to Schematic</t>
+  </si>
+  <si>
+    <t>Moving Components</t>
+  </si>
+  <si>
+    <t>Connecting Components</t>
+  </si>
+  <si>
+    <t>Labeling Components</t>
+  </si>
+  <si>
+    <t>uC Design - Microcontroller</t>
+  </si>
+  <si>
+    <t>uC Design - Reset Switch</t>
+  </si>
+  <si>
+    <t>uC Design - Oscillator</t>
+  </si>
+  <si>
+    <t>uC Design - Power Regulator</t>
+  </si>
+  <si>
+    <t>uC Design - Adding Programmer Pins</t>
+  </si>
+  <si>
+    <t>uC Design - Design Your Own</t>
+  </si>
+  <si>
+    <t>Eagle-Board</t>
+  </si>
+  <si>
+    <t>Loading Components to Board</t>
+  </si>
+  <si>
+    <t>Power Dissipating Circuit</t>
+  </si>
+  <si>
+    <t>Fuses</t>
+  </si>
+  <si>
+    <t>Common ICs</t>
+  </si>
+  <si>
+    <t>Inductors</t>
+  </si>
+  <si>
+    <t>Power Source</t>
+  </si>
+  <si>
+    <t>Voltage Nodes</t>
+  </si>
+  <si>
+    <t>Component Arrangement</t>
+  </si>
+  <si>
+    <t>Error-Checking</t>
+  </si>
+  <si>
+    <t>Silkscreen</t>
+  </si>
+  <si>
+    <t>Copper Pours</t>
+  </si>
+  <si>
+    <t>Packing and Releasing</t>
+  </si>
+  <si>
+    <t>AVR</t>
+  </si>
+  <si>
+    <t>Programming Your Board</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
@@ -346,7 +473,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -361,18 +488,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="27">
+  <borders count="31">
     <border>
       <left/>
       <right/>
@@ -638,28 +759,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top style="medium">
@@ -717,6 +816,90 @@
       <top style="medium">
         <color indexed="64"/>
       </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
       <bottom style="medium">
         <color indexed="64"/>
       </bottom>
@@ -727,7 +910,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -789,67 +972,94 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -913,7 +1123,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -946,26 +1156,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -998,23 +1191,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1194,29 +1370,29 @@
   <dimension ref="B1:F44"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="11.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="11.25" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="1.7265625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="1.7109375" style="1" customWidth="1"/>
     <col min="2" max="2" width="18" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.7265625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="11.54296875" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="9.1796875" style="1"/>
+    <col min="3" max="3" width="17.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.7109375" style="2" customWidth="1"/>
+    <col min="5" max="5" width="11.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:6" ht="11.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="2" spans="2:6" ht="11.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="28" t="s">
+      <c r="B2" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="29"/>
-      <c r="D2" s="29"/>
-      <c r="E2" s="29"/>
-      <c r="F2" s="30"/>
+      <c r="C2" s="26"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
+      <c r="F2" s="27"/>
     </row>
     <row r="3" spans="2:6" ht="11.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B3" s="9" t="s">
@@ -1273,7 +1449,7 @@
     </row>
     <row r="6" spans="2:6" ht="11.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B6" s="5" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="C6" s="3">
         <v>1</v>
@@ -1453,7 +1629,7 @@
     </row>
     <row r="16" spans="2:6" ht="11.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B16" s="5" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C16" s="3">
         <v>1</v>
@@ -1506,11 +1682,11 @@
       </c>
     </row>
     <row r="19" spans="2:6" ht="11.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B19" s="31" t="s">
+      <c r="B19" s="28" t="s">
         <v>21</v>
       </c>
-      <c r="C19" s="32"/>
-      <c r="D19" s="33"/>
+      <c r="C19" s="29"/>
+      <c r="D19" s="30"/>
       <c r="E19" s="7">
         <f>SUM(E4:E18)</f>
         <v>32.380000000000003</v>
@@ -1518,13 +1694,13 @@
       <c r="F19" s="8"/>
     </row>
     <row r="20" spans="2:6" ht="11.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B20" s="34" t="s">
+      <c r="B20" s="31" t="s">
         <v>19</v>
       </c>
-      <c r="C20" s="35"/>
-      <c r="D20" s="36"/>
-      <c r="E20" s="37"/>
-      <c r="F20" s="38"/>
+      <c r="C20" s="32"/>
+      <c r="D20" s="33"/>
+      <c r="E20" s="34"/>
+      <c r="F20" s="35"/>
     </row>
     <row r="21" spans="2:6" ht="11.25" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="22" spans="2:6" ht="11.25" customHeight="1" x14ac:dyDescent="0.35">
@@ -1535,87 +1711,87 @@
       <c r="D23" s="1"/>
       <c r="E23" s="1"/>
     </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:6" ht="11.45" x14ac:dyDescent="0.35">
       <c r="D24" s="1"/>
       <c r="E24" s="1"/>
     </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:6" ht="11.45" x14ac:dyDescent="0.35">
       <c r="D25" s="1"/>
       <c r="E25" s="1"/>
     </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:6" ht="11.45" x14ac:dyDescent="0.35">
       <c r="D26" s="1"/>
       <c r="E26" s="1"/>
     </row>
-    <row r="27" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:6" ht="11.45" x14ac:dyDescent="0.35">
       <c r="D27" s="1"/>
       <c r="E27" s="1"/>
     </row>
-    <row r="28" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="28" spans="2:6" ht="11.45" x14ac:dyDescent="0.35">
       <c r="D28" s="1"/>
       <c r="E28" s="1"/>
     </row>
-    <row r="29" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="29" spans="2:6" ht="11.45" x14ac:dyDescent="0.35">
       <c r="D29" s="1"/>
       <c r="E29" s="1"/>
     </row>
-    <row r="30" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="30" spans="2:6" ht="11.45" x14ac:dyDescent="0.35">
       <c r="D30" s="1"/>
       <c r="E30" s="1"/>
     </row>
-    <row r="31" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="31" spans="2:6" ht="11.45" x14ac:dyDescent="0.35">
       <c r="D31" s="1"/>
       <c r="E31" s="1"/>
     </row>
-    <row r="32" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="32" spans="2:6" ht="11.45" x14ac:dyDescent="0.35">
       <c r="D32" s="1"/>
       <c r="E32" s="1"/>
     </row>
-    <row r="33" spans="4:5" x14ac:dyDescent="0.35">
+    <row r="33" spans="4:5" ht="11.45" x14ac:dyDescent="0.35">
       <c r="D33" s="1"/>
       <c r="E33" s="1"/>
     </row>
-    <row r="34" spans="4:5" x14ac:dyDescent="0.35">
+    <row r="34" spans="4:5" ht="11.45" x14ac:dyDescent="0.35">
       <c r="D34" s="1"/>
       <c r="E34" s="1"/>
     </row>
-    <row r="35" spans="4:5" x14ac:dyDescent="0.35">
+    <row r="35" spans="4:5" ht="11.45" x14ac:dyDescent="0.35">
       <c r="D35" s="1"/>
       <c r="E35" s="1"/>
     </row>
-    <row r="36" spans="4:5" x14ac:dyDescent="0.35">
+    <row r="36" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D36" s="1"/>
       <c r="E36" s="1"/>
     </row>
-    <row r="37" spans="4:5" x14ac:dyDescent="0.35">
+    <row r="37" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D37" s="1"/>
       <c r="E37" s="1"/>
     </row>
-    <row r="38" spans="4:5" x14ac:dyDescent="0.35">
+    <row r="38" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D38" s="1"/>
       <c r="E38" s="1"/>
     </row>
-    <row r="39" spans="4:5" x14ac:dyDescent="0.35">
+    <row r="39" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D39" s="1"/>
       <c r="E39" s="1"/>
     </row>
-    <row r="40" spans="4:5" x14ac:dyDescent="0.35">
+    <row r="40" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D40" s="1"/>
       <c r="E40" s="1"/>
     </row>
-    <row r="41" spans="4:5" x14ac:dyDescent="0.35">
+    <row r="41" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D41" s="1"/>
       <c r="E41" s="1"/>
     </row>
-    <row r="42" spans="4:5" x14ac:dyDescent="0.35">
+    <row r="42" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D42" s="1"/>
       <c r="E42" s="1"/>
     </row>
-    <row r="43" spans="4:5" x14ac:dyDescent="0.35">
+    <row r="43" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D43" s="1"/>
       <c r="E43" s="1"/>
     </row>
-    <row r="44" spans="4:5" x14ac:dyDescent="0.35">
+    <row r="44" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D44" s="1"/>
       <c r="E44" s="1"/>
     </row>
@@ -1633,26 +1809,35 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:D63"/>
+  <dimension ref="B1:P42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="G49" sqref="G49"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q22" sqref="Q22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="11.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="11.25" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="1.7265625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="9.1796875" style="1"/>
-    <col min="3" max="3" width="37.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.1796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="9.1796875" style="1"/>
-    <col min="7" max="7" width="32.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="3" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.1796875" style="1"/>
+    <col min="1" max="1" width="1.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" style="1"/>
+    <col min="3" max="3" width="37.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="1.7109375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="9" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="37.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="1.7109375" style="1" customWidth="1"/>
+    <col min="10" max="10" width="11" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="31.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="7.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="1.7109375" style="1" customWidth="1"/>
+    <col min="14" max="14" width="10.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="27.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="7.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:4" ht="12" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="2" spans="2:4" ht="12" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="2:16" ht="12" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:16" ht="12" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="16" t="s">
         <v>56</v>
       </c>
@@ -1662,8 +1847,35 @@
       <c r="D2" s="16" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="F2" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="G2" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="H2" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="J2" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="K2" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="L2" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="N2" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="O2" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="P2" s="16" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="3" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B3" s="17" t="s">
         <v>23</v>
       </c>
@@ -1673,8 +1885,35 @@
       <c r="D3" s="17">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="F3" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="G3" s="22" t="s">
+        <v>58</v>
+      </c>
+      <c r="H3" s="13">
+        <v>0</v>
+      </c>
+      <c r="J3" s="41" t="s">
+        <v>91</v>
+      </c>
+      <c r="K3" s="41" t="s">
+        <v>92</v>
+      </c>
+      <c r="L3" s="17">
+        <v>0</v>
+      </c>
+      <c r="N3" s="41" t="s">
+        <v>123</v>
+      </c>
+      <c r="O3" s="41" t="s">
+        <v>124</v>
+      </c>
+      <c r="P3" s="17">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B4" s="14" t="s">
         <v>23</v>
       </c>
@@ -1684,8 +1923,35 @@
       <c r="D4" s="14">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="F4" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="G4" s="20" t="s">
+        <v>60</v>
+      </c>
+      <c r="H4" s="14">
+        <v>1</v>
+      </c>
+      <c r="J4" s="23" t="s">
+        <v>91</v>
+      </c>
+      <c r="K4" s="23" t="s">
+        <v>102</v>
+      </c>
+      <c r="L4" s="14">
+        <v>0</v>
+      </c>
+      <c r="N4" s="23" t="s">
+        <v>123</v>
+      </c>
+      <c r="O4" s="23" t="s">
+        <v>131</v>
+      </c>
+      <c r="P4" s="14">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B5" s="14" t="s">
         <v>23</v>
       </c>
@@ -1695,17 +1961,71 @@
       <c r="D5" s="14">
         <v>2</v>
       </c>
-    </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="F5" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="G5" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="H5" s="14">
+        <v>2</v>
+      </c>
+      <c r="J5" s="23" t="s">
+        <v>91</v>
+      </c>
+      <c r="K5" s="23" t="s">
+        <v>97</v>
+      </c>
+      <c r="L5" s="14">
+        <v>0</v>
+      </c>
+      <c r="N5" s="23" t="s">
+        <v>123</v>
+      </c>
+      <c r="O5" s="23" t="s">
+        <v>115</v>
+      </c>
+      <c r="P5" s="14">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B6" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="C6" s="21" t="s">
+      <c r="C6" s="42" t="s">
         <v>35</v>
       </c>
       <c r="D6" s="14"/>
-    </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="F6" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="G6" s="20" t="s">
+        <v>62</v>
+      </c>
+      <c r="H6" s="14">
+        <v>3</v>
+      </c>
+      <c r="J6" s="23" t="s">
+        <v>91</v>
+      </c>
+      <c r="K6" s="23" t="s">
+        <v>128</v>
+      </c>
+      <c r="L6" s="14">
+        <v>0</v>
+      </c>
+      <c r="N6" s="23" t="s">
+        <v>123</v>
+      </c>
+      <c r="O6" s="23" t="s">
+        <v>132</v>
+      </c>
+      <c r="P6" s="14">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B7" s="14" t="s">
         <v>23</v>
       </c>
@@ -1715,8 +2035,35 @@
       <c r="D7" s="14">
         <v>3</v>
       </c>
-    </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="F7" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="G7" s="20" t="s">
+        <v>63</v>
+      </c>
+      <c r="H7" s="14">
+        <v>4</v>
+      </c>
+      <c r="J7" s="23" t="s">
+        <v>91</v>
+      </c>
+      <c r="K7" s="23" t="s">
+        <v>109</v>
+      </c>
+      <c r="L7" s="14">
+        <v>0</v>
+      </c>
+      <c r="N7" s="23" t="s">
+        <v>123</v>
+      </c>
+      <c r="O7" s="23" t="s">
+        <v>134</v>
+      </c>
+      <c r="P7" s="14">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B8" s="14" t="s">
         <v>23</v>
       </c>
@@ -1726,8 +2073,33 @@
       <c r="D8" s="14">
         <v>5</v>
       </c>
-    </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="F8" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="G8" s="42" t="s">
+        <v>59</v>
+      </c>
+      <c r="H8" s="14"/>
+      <c r="J8" s="23" t="s">
+        <v>91</v>
+      </c>
+      <c r="K8" s="23" t="s">
+        <v>108</v>
+      </c>
+      <c r="L8" s="14">
+        <v>1</v>
+      </c>
+      <c r="N8" s="23" t="s">
+        <v>123</v>
+      </c>
+      <c r="O8" s="23" t="s">
+        <v>133</v>
+      </c>
+      <c r="P8" s="14">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B9" s="14" t="s">
         <v>23</v>
       </c>
@@ -1737,26 +2109,94 @@
       <c r="D9" s="14">
         <v>6</v>
       </c>
-    </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="F9" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="G9" s="20" t="s">
+        <v>64</v>
+      </c>
+      <c r="H9" s="14">
+        <v>5</v>
+      </c>
+      <c r="J9" s="23" t="s">
+        <v>91</v>
+      </c>
+      <c r="K9" s="23" t="s">
+        <v>93</v>
+      </c>
+      <c r="L9" s="14">
+        <v>1</v>
+      </c>
+      <c r="N9" s="23" t="s">
+        <v>123</v>
+      </c>
+      <c r="O9" s="23" t="s">
+        <v>135</v>
+      </c>
+      <c r="P9" s="14">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="2:16" ht="12" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B10" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="C10" s="21" t="s">
+      <c r="C10" s="42" t="s">
         <v>37</v>
       </c>
       <c r="D10" s="14"/>
-    </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="F10" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="G10" s="20" t="s">
+        <v>65</v>
+      </c>
+      <c r="H10" s="14">
+        <v>6</v>
+      </c>
+      <c r="J10" s="23" t="s">
+        <v>91</v>
+      </c>
+      <c r="K10" s="23" t="s">
+        <v>94</v>
+      </c>
+      <c r="L10" s="14">
+        <v>1</v>
+      </c>
+      <c r="N10" s="46" t="s">
+        <v>123</v>
+      </c>
+      <c r="O10" s="47" t="s">
+        <v>122</v>
+      </c>
+      <c r="P10" s="15"/>
+    </row>
+    <row r="11" spans="2:16" ht="12" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B11" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="C11" s="21" t="s">
+      <c r="C11" s="42" t="s">
         <v>41</v>
       </c>
       <c r="D11" s="14"/>
-    </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="F11" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="G11" s="42" t="s">
+        <v>66</v>
+      </c>
+      <c r="H11" s="14"/>
+      <c r="J11" s="23" t="s">
+        <v>91</v>
+      </c>
+      <c r="K11" s="23" t="s">
+        <v>126</v>
+      </c>
+      <c r="L11" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="2:16" ht="12" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B12" s="14" t="s">
         <v>23</v>
       </c>
@@ -1766,17 +2206,69 @@
       <c r="D12" s="14">
         <v>7</v>
       </c>
-    </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="F12" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="G12" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="H12" s="14">
+        <v>7</v>
+      </c>
+      <c r="J12" s="23" t="s">
+        <v>91</v>
+      </c>
+      <c r="K12" s="23" t="s">
+        <v>96</v>
+      </c>
+      <c r="L12" s="14">
+        <v>2</v>
+      </c>
+      <c r="N12" s="38" t="s">
+        <v>56</v>
+      </c>
+      <c r="O12" s="39" t="s">
+        <v>22</v>
+      </c>
+      <c r="P12" s="40" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="13" spans="2:16" ht="12" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B13" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="C13" s="21" t="s">
+      <c r="C13" s="42" t="s">
         <v>49</v>
       </c>
       <c r="D13" s="14"/>
-    </row>
-    <row r="14" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="F13" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="G13" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="H13" s="14">
+        <v>8</v>
+      </c>
+      <c r="J13" s="23" t="s">
+        <v>91</v>
+      </c>
+      <c r="K13" s="23" t="s">
+        <v>95</v>
+      </c>
+      <c r="L13" s="14">
+        <v>2</v>
+      </c>
+      <c r="N13" s="48" t="s">
+        <v>136</v>
+      </c>
+      <c r="O13" s="49" t="s">
+        <v>137</v>
+      </c>
+      <c r="P13" s="50"/>
+    </row>
+    <row r="14" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B14" s="14" t="s">
         <v>23</v>
       </c>
@@ -1786,26 +2278,78 @@
       <c r="D14" s="14">
         <v>8</v>
       </c>
-    </row>
-    <row r="15" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="F14" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="G14" s="42" t="s">
+        <v>67</v>
+      </c>
+      <c r="H14" s="14"/>
+      <c r="J14" s="23" t="s">
+        <v>91</v>
+      </c>
+      <c r="K14" s="23" t="s">
+        <v>98</v>
+      </c>
+      <c r="L14" s="14">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B15" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="C15" s="21" t="s">
+      <c r="C15" s="42" t="s">
         <v>50</v>
       </c>
       <c r="D15" s="14"/>
-    </row>
-    <row r="16" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="F15" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="G15" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="H15" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="J15" s="23" t="s">
+        <v>91</v>
+      </c>
+      <c r="K15" s="23" t="s">
+        <v>99</v>
+      </c>
+      <c r="L15" s="14">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B16" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="C16" s="21" t="s">
+      <c r="C16" s="42" t="s">
         <v>51</v>
       </c>
       <c r="D16" s="14"/>
-    </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="F16" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="G16" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="H16" s="14" t="s">
+        <v>76</v>
+      </c>
+      <c r="J16" s="23" t="s">
+        <v>91</v>
+      </c>
+      <c r="K16" s="23" t="s">
+        <v>127</v>
+      </c>
+      <c r="L16" s="14">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B17" s="14" t="s">
         <v>23</v>
       </c>
@@ -1815,17 +2359,53 @@
       <c r="D17" s="14">
         <v>9</v>
       </c>
-    </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="F17" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="G17" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="H17" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="J17" s="23" t="s">
+        <v>91</v>
+      </c>
+      <c r="K17" s="23" t="s">
+        <v>129</v>
+      </c>
+      <c r="L17" s="14">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="2:12" ht="12" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B18" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="C18" s="21" t="s">
+      <c r="C18" s="42" t="s">
         <v>52</v>
       </c>
       <c r="D18" s="14"/>
-    </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="F18" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="G18" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="H18" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="J18" s="36" t="s">
+        <v>91</v>
+      </c>
+      <c r="K18" s="36" t="s">
+        <v>130</v>
+      </c>
+      <c r="L18" s="15">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="2:12" ht="12" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B19" s="14" t="s">
         <v>23</v>
       </c>
@@ -1835,17 +2415,44 @@
       <c r="D19" s="14">
         <v>10</v>
       </c>
-    </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="F19" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="G19" s="42" t="s">
+        <v>48</v>
+      </c>
+      <c r="H19" s="14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="20" spans="2:12" ht="12" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B20" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="C20" s="21" t="s">
+      <c r="C20" s="42" t="s">
         <v>53</v>
       </c>
       <c r="D20" s="14"/>
-    </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="F20" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="G20" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="H20" s="14">
+        <v>12</v>
+      </c>
+      <c r="J20" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="K20" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="L20" s="16" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="21" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B21" s="14" t="s">
         <v>23</v>
       </c>
@@ -1855,17 +2462,53 @@
       <c r="D21" s="14">
         <v>11</v>
       </c>
-    </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="F21" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="G21" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="H21" s="14">
+        <v>13</v>
+      </c>
+      <c r="J21" s="41" t="s">
+        <v>100</v>
+      </c>
+      <c r="K21" s="41" t="s">
+        <v>103</v>
+      </c>
+      <c r="L21" s="17">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B22" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="C22" s="21" t="s">
+      <c r="C22" s="42" t="s">
         <v>54</v>
       </c>
       <c r="D22" s="14"/>
-    </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="F22" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="G22" s="20" t="s">
+        <v>44</v>
+      </c>
+      <c r="H22" s="14">
+        <v>14</v>
+      </c>
+      <c r="J22" s="23" t="s">
+        <v>100</v>
+      </c>
+      <c r="K22" s="23" t="s">
+        <v>104</v>
+      </c>
+      <c r="L22" s="14">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B23" s="14" t="s">
         <v>23</v>
       </c>
@@ -1875,428 +2518,356 @@
       <c r="D23" s="14">
         <v>4</v>
       </c>
-    </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="F23" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="G23" s="20" t="s">
+        <v>45</v>
+      </c>
+      <c r="H23" s="14">
+        <v>15</v>
+      </c>
+      <c r="J23" s="23" t="s">
+        <v>100</v>
+      </c>
+      <c r="K23" s="23" t="s">
+        <v>105</v>
+      </c>
+      <c r="L23" s="14">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B24" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="C24" s="22" t="s">
+      <c r="C24" s="21" t="s">
         <v>70</v>
       </c>
       <c r="D24" s="14">
         <v>12</v>
       </c>
-    </row>
-    <row r="25" spans="2:4" ht="12" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B25" s="24" t="s">
+      <c r="F24" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="G24" s="20" t="s">
+        <v>46</v>
+      </c>
+      <c r="H24" s="14" t="s">
+        <v>86</v>
+      </c>
+      <c r="J24" s="23" t="s">
+        <v>100</v>
+      </c>
+      <c r="K24" s="23" t="s">
+        <v>101</v>
+      </c>
+      <c r="L24" s="14">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="25" spans="2:12" ht="12" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B25" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="C25" s="25" t="s">
+      <c r="C25" s="37" t="s">
         <v>74</v>
       </c>
-      <c r="D25" s="24">
+      <c r="D25" s="15">
         <v>13</v>
       </c>
-    </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B26" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="C26" s="26" t="s">
-        <v>58</v>
-      </c>
-      <c r="D26" s="13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B27" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="C27" s="20" t="s">
-        <v>60</v>
-      </c>
-      <c r="D27" s="14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B28" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="C28" s="20" t="s">
-        <v>61</v>
-      </c>
-      <c r="D28" s="14">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="29" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B29" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="C29" s="20" t="s">
-        <v>62</v>
-      </c>
-      <c r="D29" s="14">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B30" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="C30" s="20" t="s">
-        <v>63</v>
-      </c>
-      <c r="D30" s="14">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="31" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B31" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="C31" s="21" t="s">
-        <v>59</v>
-      </c>
-      <c r="D31" s="14"/>
-    </row>
-    <row r="32" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B32" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="C32" s="20" t="s">
-        <v>64</v>
-      </c>
-      <c r="D32" s="14">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B33" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="C33" s="20" t="s">
-        <v>65</v>
-      </c>
-      <c r="D33" s="14">
+      <c r="F25" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="G25" s="20" t="s">
+        <v>46</v>
+      </c>
+      <c r="H25" s="14" t="s">
+        <v>85</v>
+      </c>
+      <c r="J25" s="36" t="s">
+        <v>100</v>
+      </c>
+      <c r="K25" s="36" t="s">
+        <v>106</v>
+      </c>
+      <c r="L25" s="15">
         <v>6</v>
       </c>
     </row>
-    <row r="34" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B34" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="C34" s="21" t="s">
-        <v>66</v>
-      </c>
-      <c r="D34" s="14"/>
-    </row>
-    <row r="35" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B35" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="C35" s="20" t="s">
-        <v>32</v>
-      </c>
-      <c r="D35" s="14">
+    <row r="26" spans="2:12" ht="12" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F26" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="G26" s="42" t="s">
+        <v>80</v>
+      </c>
+      <c r="H26" s="14"/>
+    </row>
+    <row r="27" spans="2:12" ht="12" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F27" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="G27" s="20" t="s">
+        <v>79</v>
+      </c>
+      <c r="H27" s="14">
+        <v>22</v>
+      </c>
+      <c r="J27" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="K27" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="L27" s="16" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="28" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="F28" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="G28" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="H28" s="14">
+        <v>23</v>
+      </c>
+      <c r="J28" s="41" t="s">
+        <v>107</v>
+      </c>
+      <c r="K28" s="41" t="s">
+        <v>113</v>
+      </c>
+      <c r="L28" s="17">
         <v>7</v>
       </c>
     </row>
-    <row r="36" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B36" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="C36" s="20" t="s">
-        <v>36</v>
-      </c>
-      <c r="D36" s="14">
+    <row r="29" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="F29" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="G29" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="H29" s="14">
+        <v>9</v>
+      </c>
+      <c r="J29" s="23" t="s">
+        <v>107</v>
+      </c>
+      <c r="K29" s="23" t="s">
+        <v>116</v>
+      </c>
+      <c r="L29" s="14">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="30" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="F30" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="G30" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="H30" s="14">
+        <v>10</v>
+      </c>
+      <c r="J30" s="23" t="s">
+        <v>107</v>
+      </c>
+      <c r="K30" s="23" t="s">
+        <v>114</v>
+      </c>
+      <c r="L30" s="14">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="31" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="F31" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="G31" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="H31" s="14">
+        <v>11</v>
+      </c>
+      <c r="J31" s="23" t="s">
+        <v>107</v>
+      </c>
+      <c r="K31" s="23" t="s">
+        <v>115</v>
+      </c>
+      <c r="L31" s="14">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="32" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="F32" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="G32" s="42" t="s">
+        <v>81</v>
+      </c>
+      <c r="H32" s="14"/>
+      <c r="J32" s="23" t="s">
+        <v>107</v>
+      </c>
+      <c r="K32" s="23" t="s">
+        <v>125</v>
+      </c>
+      <c r="L32" s="14">
         <v>8</v>
       </c>
     </row>
-    <row r="37" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B37" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="C37" s="21" t="s">
-        <v>67</v>
-      </c>
-      <c r="D37" s="14"/>
-    </row>
-    <row r="38" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B38" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="C38" s="20" t="s">
-        <v>47</v>
-      </c>
-      <c r="D38" s="14" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="39" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B39" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="C39" s="20" t="s">
-        <v>47</v>
-      </c>
-      <c r="D39" s="14" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="40" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B40" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="C40" s="20" t="s">
-        <v>47</v>
-      </c>
-      <c r="D40" s="14" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="41" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B41" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="C41" s="20" t="s">
-        <v>48</v>
-      </c>
-      <c r="D41" s="14" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="42" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B42" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="C42" s="21" t="s">
-        <v>48</v>
-      </c>
-      <c r="D42" s="14" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="43" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B43" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="C43" s="20" t="s">
-        <v>42</v>
-      </c>
-      <c r="D43" s="14">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="44" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B44" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="C44" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="D44" s="14">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="45" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B45" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="C45" s="20" t="s">
-        <v>44</v>
-      </c>
-      <c r="D45" s="14">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="46" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B46" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="C46" s="20" t="s">
-        <v>45</v>
-      </c>
-      <c r="D46" s="14">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="47" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B47" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="C47" s="20" t="s">
-        <v>46</v>
-      </c>
-      <c r="D47" s="14" t="s">
+    <row r="33" spans="6:12" x14ac:dyDescent="0.25">
+      <c r="F33" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="G33" s="20" t="s">
+        <v>71</v>
+      </c>
+      <c r="H33" s="14">
+        <v>19</v>
+      </c>
+      <c r="J33" s="44" t="s">
+        <v>107</v>
+      </c>
+      <c r="K33" s="45" t="s">
+        <v>110</v>
+      </c>
+      <c r="L33" s="14"/>
+    </row>
+    <row r="34" spans="6:12" x14ac:dyDescent="0.25">
+      <c r="F34" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="G34" s="20" t="s">
+        <v>72</v>
+      </c>
+      <c r="H34" s="23" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="48" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B48" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="C48" s="20" t="s">
-        <v>46</v>
-      </c>
-      <c r="D48" s="14" t="s">
+      <c r="J34" s="23" t="s">
+        <v>107</v>
+      </c>
+      <c r="K34" s="23" t="s">
+        <v>111</v>
+      </c>
+      <c r="L34" s="23">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="35" spans="6:12" x14ac:dyDescent="0.25">
+      <c r="F35" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="G35" s="24" t="s">
+        <v>73</v>
+      </c>
+      <c r="H35" s="23" t="s">
+        <v>90</v>
+      </c>
+      <c r="J35" s="23" t="s">
+        <v>107</v>
+      </c>
+      <c r="K35" s="23" t="s">
+        <v>111</v>
+      </c>
+      <c r="L35" s="23">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="36" spans="6:12" x14ac:dyDescent="0.25">
+      <c r="F36" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="G36" s="24" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="49" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B49" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="C49" s="21" t="s">
-        <v>80</v>
-      </c>
-      <c r="D49" s="14"/>
-    </row>
-    <row r="50" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B50" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="C50" s="20" t="s">
-        <v>79</v>
-      </c>
-      <c r="D50" s="14">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="51" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B51" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="C51" s="20" t="s">
-        <v>17</v>
-      </c>
-      <c r="D51" s="14">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="52" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B52" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="C52" s="20" t="s">
-        <v>38</v>
-      </c>
-      <c r="D52" s="14">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="53" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B53" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="C53" s="20" t="s">
-        <v>39</v>
-      </c>
-      <c r="D53" s="14">
+      <c r="H36" s="14">
+        <v>21</v>
+      </c>
+      <c r="J36" s="44" t="s">
+        <v>107</v>
+      </c>
+      <c r="K36" s="45" t="s">
+        <v>112</v>
+      </c>
+      <c r="L36" s="14"/>
+    </row>
+    <row r="37" spans="6:12" ht="12" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F37" s="36" t="s">
+        <v>24</v>
+      </c>
+      <c r="G37" s="43" t="s">
+        <v>87</v>
+      </c>
+      <c r="H37" s="15"/>
+      <c r="J37" s="23" t="s">
+        <v>107</v>
+      </c>
+      <c r="K37" s="23" t="s">
+        <v>117</v>
+      </c>
+      <c r="L37" s="14">
         <v>10</v>
       </c>
     </row>
-    <row r="54" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B54" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="C54" s="20" t="s">
-        <v>40</v>
-      </c>
-      <c r="D54" s="14">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="55" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B55" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="C55" s="21" t="s">
-        <v>81</v>
-      </c>
-      <c r="D55" s="14"/>
-    </row>
-    <row r="56" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B56" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="C56" s="20" t="s">
-        <v>71</v>
-      </c>
-      <c r="D56" s="14">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="57" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B57" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="C57" s="20" t="s">
-        <v>72</v>
-      </c>
-      <c r="D57" s="39" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="58" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B58" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="C58" s="40" t="s">
-        <v>73</v>
-      </c>
-      <c r="D58" s="39" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="59" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B59" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="C59" s="40" t="s">
-        <v>91</v>
-      </c>
-      <c r="D59" s="14">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="60" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B60" s="39" t="s">
-        <v>24</v>
-      </c>
-      <c r="C60" s="41" t="s">
-        <v>90</v>
-      </c>
-      <c r="D60" s="14"/>
-    </row>
-    <row r="61" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B61" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="C61" s="23" t="s">
-        <v>82</v>
-      </c>
-      <c r="D61" s="14"/>
-    </row>
-    <row r="62" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B62" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="C62" s="22" t="s">
-        <v>84</v>
-      </c>
-      <c r="D62" s="14"/>
-    </row>
-    <row r="63" spans="2:4" ht="12" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B63" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="C63" s="27" t="s">
-        <v>85</v>
-      </c>
-      <c r="D63" s="15"/>
+    <row r="38" spans="6:12" x14ac:dyDescent="0.25">
+      <c r="J38" s="23" t="s">
+        <v>107</v>
+      </c>
+      <c r="K38" s="23" t="s">
+        <v>119</v>
+      </c>
+      <c r="L38" s="14">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="39" spans="6:12" x14ac:dyDescent="0.25">
+      <c r="J39" s="23" t="s">
+        <v>107</v>
+      </c>
+      <c r="K39" s="23" t="s">
+        <v>118</v>
+      </c>
+      <c r="L39" s="14">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="40" spans="6:12" x14ac:dyDescent="0.25">
+      <c r="J40" s="23" t="s">
+        <v>107</v>
+      </c>
+      <c r="K40" s="23" t="s">
+        <v>120</v>
+      </c>
+      <c r="L40" s="14">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="41" spans="6:12" x14ac:dyDescent="0.25">
+      <c r="J41" s="23" t="s">
+        <v>107</v>
+      </c>
+      <c r="K41" s="23" t="s">
+        <v>121</v>
+      </c>
+      <c r="L41" s="14">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="42" spans="6:12" ht="12" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J42" s="46" t="s">
+        <v>107</v>
+      </c>
+      <c r="K42" s="47" t="s">
+        <v>122</v>
+      </c>
+      <c r="L42" s="15"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added Works_001 for Eagle CAD
</commit_message>
<xml_diff>
--- a/Workshop_Materials.xlsx
+++ b/Workshop_Materials.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="139">
   <si>
     <t>List of Components</t>
   </si>
@@ -302,9 +302,6 @@
     <t>Buttons</t>
   </si>
   <si>
-    <t>Transistors/MOSFET</t>
-  </si>
-  <si>
     <t>Relays</t>
   </si>
   <si>
@@ -392,9 +389,6 @@
     <t>Loading Components to Board</t>
   </si>
   <si>
-    <t>Power Dissipating Circuit</t>
-  </si>
-  <si>
     <t>Fuses</t>
   </si>
   <si>
@@ -429,6 +423,15 @@
   </si>
   <si>
     <t>Programming Your Board</t>
+  </si>
+  <si>
+    <t>H-Bridge</t>
+  </si>
+  <si>
+    <t>Deboupling Circuit</t>
+  </si>
+  <si>
+    <t>BJT/MOSFET</t>
   </si>
 </sst>
 </file>
@@ -984,6 +987,51 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1015,51 +1063,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1386,13 +1389,13 @@
   <sheetData>
     <row r="1" spans="2:6" ht="11.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="2" spans="2:6" ht="11.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="25" t="s">
+      <c r="B2" s="40" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="26"/>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26"/>
-      <c r="F2" s="27"/>
+      <c r="C2" s="41"/>
+      <c r="D2" s="41"/>
+      <c r="E2" s="41"/>
+      <c r="F2" s="42"/>
     </row>
     <row r="3" spans="2:6" ht="11.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B3" s="9" t="s">
@@ -1682,11 +1685,11 @@
       </c>
     </row>
     <row r="19" spans="2:6" ht="11.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B19" s="28" t="s">
+      <c r="B19" s="43" t="s">
         <v>21</v>
       </c>
-      <c r="C19" s="29"/>
-      <c r="D19" s="30"/>
+      <c r="C19" s="44"/>
+      <c r="D19" s="45"/>
       <c r="E19" s="7">
         <f>SUM(E4:E18)</f>
         <v>32.380000000000003</v>
@@ -1694,13 +1697,13 @@
       <c r="F19" s="8"/>
     </row>
     <row r="20" spans="2:6" ht="11.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B20" s="31" t="s">
+      <c r="B20" s="46" t="s">
         <v>19</v>
       </c>
-      <c r="C20" s="32"/>
-      <c r="D20" s="33"/>
-      <c r="E20" s="34"/>
-      <c r="F20" s="35"/>
+      <c r="C20" s="47"/>
+      <c r="D20" s="48"/>
+      <c r="E20" s="49"/>
+      <c r="F20" s="50"/>
     </row>
     <row r="21" spans="2:6" ht="11.25" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="22" spans="2:6" ht="11.25" customHeight="1" x14ac:dyDescent="0.35">
@@ -1809,10 +1812,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:P42"/>
+  <dimension ref="B1:P43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q22" sqref="Q22"/>
+      <selection activeCell="P26" sqref="P26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="11.25" x14ac:dyDescent="0.25"/>
@@ -1894,20 +1897,20 @@
       <c r="H3" s="13">
         <v>0</v>
       </c>
-      <c r="J3" s="41" t="s">
+      <c r="J3" s="30" t="s">
         <v>91</v>
       </c>
-      <c r="K3" s="41" t="s">
+      <c r="K3" s="30" t="s">
         <v>92</v>
       </c>
       <c r="L3" s="17">
         <v>0</v>
       </c>
-      <c r="N3" s="41" t="s">
+      <c r="N3" s="30" t="s">
+        <v>122</v>
+      </c>
+      <c r="O3" s="30" t="s">
         <v>123</v>
-      </c>
-      <c r="O3" s="41" t="s">
-        <v>124</v>
       </c>
       <c r="P3" s="17">
         <v>10</v>
@@ -1936,16 +1939,16 @@
         <v>91</v>
       </c>
       <c r="K4" s="23" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="L4" s="14">
         <v>0</v>
       </c>
       <c r="N4" s="23" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="O4" s="23" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="P4" s="14">
         <v>10</v>
@@ -1974,16 +1977,16 @@
         <v>91</v>
       </c>
       <c r="K5" s="23" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="L5" s="14">
         <v>0</v>
       </c>
       <c r="N5" s="23" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="O5" s="23" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="P5" s="14">
         <v>10</v>
@@ -1993,7 +1996,7 @@
       <c r="B6" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="C6" s="42" t="s">
+      <c r="C6" s="31" t="s">
         <v>35</v>
       </c>
       <c r="D6" s="14"/>
@@ -2010,16 +2013,16 @@
         <v>91</v>
       </c>
       <c r="K6" s="23" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="L6" s="14">
         <v>0</v>
       </c>
       <c r="N6" s="23" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="O6" s="23" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="P6" s="14">
         <v>10</v>
@@ -2048,16 +2051,16 @@
         <v>91</v>
       </c>
       <c r="K7" s="23" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="L7" s="14">
         <v>0</v>
       </c>
       <c r="N7" s="23" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="O7" s="23" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="P7" s="14">
         <v>10</v>
@@ -2076,7 +2079,7 @@
       <c r="F8" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="G8" s="42" t="s">
+      <c r="G8" s="31" t="s">
         <v>59</v>
       </c>
       <c r="H8" s="14"/>
@@ -2084,16 +2087,16 @@
         <v>91</v>
       </c>
       <c r="K8" s="23" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="L8" s="14">
         <v>1</v>
       </c>
       <c r="N8" s="23" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="O8" s="23" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="P8" s="14">
         <v>10</v>
@@ -2128,10 +2131,10 @@
         <v>1</v>
       </c>
       <c r="N9" s="23" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="O9" s="23" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="P9" s="14">
         <v>10</v>
@@ -2141,7 +2144,7 @@
       <c r="B10" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="C10" s="42" t="s">
+      <c r="C10" s="31" t="s">
         <v>37</v>
       </c>
       <c r="D10" s="14"/>
@@ -2163,11 +2166,11 @@
       <c r="L10" s="14">
         <v>1</v>
       </c>
-      <c r="N10" s="46" t="s">
-        <v>123</v>
-      </c>
-      <c r="O10" s="47" t="s">
+      <c r="N10" s="35" t="s">
         <v>122</v>
+      </c>
+      <c r="O10" s="36" t="s">
+        <v>121</v>
       </c>
       <c r="P10" s="15"/>
     </row>
@@ -2175,14 +2178,14 @@
       <c r="B11" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="C11" s="42" t="s">
+      <c r="C11" s="31" t="s">
         <v>41</v>
       </c>
       <c r="D11" s="14"/>
       <c r="F11" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="G11" s="42" t="s">
+      <c r="G11" s="31" t="s">
         <v>66</v>
       </c>
       <c r="H11" s="14"/>
@@ -2190,7 +2193,7 @@
         <v>91</v>
       </c>
       <c r="K11" s="23" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="L11" s="14">
         <v>1</v>
@@ -2219,18 +2222,18 @@
         <v>91</v>
       </c>
       <c r="K12" s="23" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="L12" s="14">
         <v>2</v>
       </c>
-      <c r="N12" s="38" t="s">
+      <c r="N12" s="27" t="s">
         <v>56</v>
       </c>
-      <c r="O12" s="39" t="s">
+      <c r="O12" s="28" t="s">
         <v>22</v>
       </c>
-      <c r="P12" s="40" t="s">
+      <c r="P12" s="29" t="s">
         <v>55</v>
       </c>
     </row>
@@ -2238,7 +2241,7 @@
       <c r="B13" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="C13" s="42" t="s">
+      <c r="C13" s="31" t="s">
         <v>49</v>
       </c>
       <c r="D13" s="14"/>
@@ -2255,18 +2258,18 @@
         <v>91</v>
       </c>
       <c r="K13" s="23" t="s">
-        <v>95</v>
+        <v>138</v>
       </c>
       <c r="L13" s="14">
         <v>2</v>
       </c>
-      <c r="N13" s="48" t="s">
-        <v>136</v>
-      </c>
-      <c r="O13" s="49" t="s">
-        <v>137</v>
-      </c>
-      <c r="P13" s="50"/>
+      <c r="N13" s="37" t="s">
+        <v>134</v>
+      </c>
+      <c r="O13" s="38" t="s">
+        <v>135</v>
+      </c>
+      <c r="P13" s="39"/>
     </row>
     <row r="14" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B14" s="14" t="s">
@@ -2281,7 +2284,7 @@
       <c r="F14" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="G14" s="42" t="s">
+      <c r="G14" s="31" t="s">
         <v>67</v>
       </c>
       <c r="H14" s="14"/>
@@ -2289,7 +2292,7 @@
         <v>91</v>
       </c>
       <c r="K14" s="23" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="L14" s="14">
         <v>2</v>
@@ -2299,7 +2302,7 @@
       <c r="B15" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="C15" s="42" t="s">
+      <c r="C15" s="31" t="s">
         <v>50</v>
       </c>
       <c r="D15" s="14"/>
@@ -2316,7 +2319,7 @@
         <v>91</v>
       </c>
       <c r="K15" s="23" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="L15" s="14">
         <v>3</v>
@@ -2326,7 +2329,7 @@
       <c r="B16" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="C16" s="42" t="s">
+      <c r="C16" s="31" t="s">
         <v>51</v>
       </c>
       <c r="D16" s="14"/>
@@ -2343,7 +2346,7 @@
         <v>91</v>
       </c>
       <c r="K16" s="23" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="L16" s="14">
         <v>4</v>
@@ -2372,7 +2375,7 @@
         <v>91</v>
       </c>
       <c r="K17" s="23" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="L17" s="14">
         <v>5</v>
@@ -2382,7 +2385,7 @@
       <c r="B18" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="C18" s="42" t="s">
+      <c r="C18" s="31" t="s">
         <v>52</v>
       </c>
       <c r="D18" s="14"/>
@@ -2395,11 +2398,11 @@
       <c r="H18" s="14" t="s">
         <v>77</v>
       </c>
-      <c r="J18" s="36" t="s">
+      <c r="J18" s="25" t="s">
         <v>91</v>
       </c>
-      <c r="K18" s="36" t="s">
-        <v>130</v>
+      <c r="K18" s="25" t="s">
+        <v>128</v>
       </c>
       <c r="L18" s="15">
         <v>5</v>
@@ -2418,7 +2421,7 @@
       <c r="F19" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="G19" s="42" t="s">
+      <c r="G19" s="31" t="s">
         <v>48</v>
       </c>
       <c r="H19" s="14" t="s">
@@ -2429,7 +2432,7 @@
       <c r="B20" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="C20" s="42" t="s">
+      <c r="C20" s="31" t="s">
         <v>53</v>
       </c>
       <c r="D20" s="14"/>
@@ -2471,11 +2474,11 @@
       <c r="H21" s="14">
         <v>13</v>
       </c>
-      <c r="J21" s="41" t="s">
-        <v>100</v>
-      </c>
-      <c r="K21" s="41" t="s">
-        <v>103</v>
+      <c r="J21" s="30" t="s">
+        <v>99</v>
+      </c>
+      <c r="K21" s="30" t="s">
+        <v>102</v>
       </c>
       <c r="L21" s="17">
         <v>5</v>
@@ -2485,7 +2488,7 @@
       <c r="B22" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="C22" s="42" t="s">
+      <c r="C22" s="31" t="s">
         <v>54</v>
       </c>
       <c r="D22" s="14"/>
@@ -2499,10 +2502,10 @@
         <v>14</v>
       </c>
       <c r="J22" s="23" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="K22" s="23" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="L22" s="14">
         <v>5</v>
@@ -2528,10 +2531,10 @@
         <v>15</v>
       </c>
       <c r="J23" s="23" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="K23" s="23" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="L23" s="14">
         <v>5</v>
@@ -2557,10 +2560,10 @@
         <v>86</v>
       </c>
       <c r="J24" s="23" t="s">
+        <v>99</v>
+      </c>
+      <c r="K24" s="23" t="s">
         <v>100</v>
-      </c>
-      <c r="K24" s="23" t="s">
-        <v>101</v>
       </c>
       <c r="L24" s="14">
         <v>5</v>
@@ -2570,7 +2573,7 @@
       <c r="B25" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="C25" s="37" t="s">
+      <c r="C25" s="26" t="s">
         <v>74</v>
       </c>
       <c r="D25" s="15">
@@ -2585,13 +2588,13 @@
       <c r="H25" s="14" t="s">
         <v>85</v>
       </c>
-      <c r="J25" s="36" t="s">
-        <v>100</v>
-      </c>
-      <c r="K25" s="36" t="s">
-        <v>106</v>
-      </c>
-      <c r="L25" s="15">
+      <c r="J25" s="23" t="s">
+        <v>99</v>
+      </c>
+      <c r="K25" s="23" t="s">
+        <v>136</v>
+      </c>
+      <c r="L25" s="14">
         <v>6</v>
       </c>
     </row>
@@ -2599,10 +2602,19 @@
       <c r="F26" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="G26" s="42" t="s">
+      <c r="G26" s="31" t="s">
         <v>80</v>
       </c>
       <c r="H26" s="14"/>
+      <c r="J26" s="25" t="s">
+        <v>99</v>
+      </c>
+      <c r="K26" s="25" t="s">
+        <v>105</v>
+      </c>
+      <c r="L26" s="15">
+        <v>6</v>
+      </c>
     </row>
     <row r="27" spans="2:12" ht="12" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F27" s="14" t="s">
@@ -2614,17 +2626,8 @@
       <c r="H27" s="14">
         <v>22</v>
       </c>
-      <c r="J27" s="16" t="s">
-        <v>56</v>
-      </c>
-      <c r="K27" s="16" t="s">
-        <v>22</v>
-      </c>
-      <c r="L27" s="16" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="28" spans="2:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="28" spans="2:12" ht="12" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F28" s="14" t="s">
         <v>24</v>
       </c>
@@ -2634,14 +2637,14 @@
       <c r="H28" s="14">
         <v>23</v>
       </c>
-      <c r="J28" s="41" t="s">
-        <v>107</v>
-      </c>
-      <c r="K28" s="41" t="s">
-        <v>113</v>
-      </c>
-      <c r="L28" s="17">
-        <v>7</v>
+      <c r="J28" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="K28" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="L28" s="16" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="29" spans="2:12" x14ac:dyDescent="0.25">
@@ -2654,13 +2657,13 @@
       <c r="H29" s="14">
         <v>9</v>
       </c>
-      <c r="J29" s="23" t="s">
-        <v>107</v>
-      </c>
-      <c r="K29" s="23" t="s">
-        <v>116</v>
-      </c>
-      <c r="L29" s="14">
+      <c r="J29" s="30" t="s">
+        <v>106</v>
+      </c>
+      <c r="K29" s="30" t="s">
+        <v>112</v>
+      </c>
+      <c r="L29" s="17">
         <v>7</v>
       </c>
     </row>
@@ -2675,10 +2678,10 @@
         <v>10</v>
       </c>
       <c r="J30" s="23" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="K30" s="23" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="L30" s="14">
         <v>7</v>
@@ -2695,10 +2698,10 @@
         <v>11</v>
       </c>
       <c r="J31" s="23" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="K31" s="23" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="L31" s="14">
         <v>7</v>
@@ -2708,18 +2711,18 @@
       <c r="F32" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="G32" s="42" t="s">
+      <c r="G32" s="31" t="s">
         <v>81</v>
       </c>
       <c r="H32" s="14"/>
       <c r="J32" s="23" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="K32" s="23" t="s">
-        <v>125</v>
+        <v>114</v>
       </c>
       <c r="L32" s="14">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="33" spans="6:12" x14ac:dyDescent="0.25">
@@ -2732,13 +2735,15 @@
       <c r="H33" s="14">
         <v>19</v>
       </c>
-      <c r="J33" s="44" t="s">
-        <v>107</v>
-      </c>
-      <c r="K33" s="45" t="s">
-        <v>110</v>
-      </c>
-      <c r="L33" s="14"/>
+      <c r="J33" s="23" t="s">
+        <v>106</v>
+      </c>
+      <c r="K33" s="23" t="s">
+        <v>137</v>
+      </c>
+      <c r="L33" s="14">
+        <v>7</v>
+      </c>
     </row>
     <row r="34" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F34" s="14" t="s">
@@ -2750,15 +2755,13 @@
       <c r="H34" s="23" t="s">
         <v>89</v>
       </c>
-      <c r="J34" s="23" t="s">
-        <v>107</v>
-      </c>
-      <c r="K34" s="23" t="s">
-        <v>111</v>
-      </c>
-      <c r="L34" s="23">
-        <v>9</v>
-      </c>
+      <c r="J34" s="33" t="s">
+        <v>106</v>
+      </c>
+      <c r="K34" s="34" t="s">
+        <v>109</v>
+      </c>
+      <c r="L34" s="14"/>
     </row>
     <row r="35" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F35" s="14" t="s">
@@ -2771,13 +2774,13 @@
         <v>90</v>
       </c>
       <c r="J35" s="23" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="K35" s="23" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="L35" s="23">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="36" spans="6:12" x14ac:dyDescent="0.25">
@@ -2790,84 +2793,95 @@
       <c r="H36" s="14">
         <v>21</v>
       </c>
-      <c r="J36" s="44" t="s">
-        <v>107</v>
-      </c>
-      <c r="K36" s="45" t="s">
-        <v>112</v>
-      </c>
-      <c r="L36" s="14"/>
+      <c r="J36" s="23" t="s">
+        <v>106</v>
+      </c>
+      <c r="K36" s="23" t="s">
+        <v>110</v>
+      </c>
+      <c r="L36" s="23">
+        <v>8</v>
+      </c>
     </row>
     <row r="37" spans="6:12" ht="12" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F37" s="36" t="s">
-        <v>24</v>
-      </c>
-      <c r="G37" s="43" t="s">
+      <c r="F37" s="25" t="s">
+        <v>24</v>
+      </c>
+      <c r="G37" s="32" t="s">
         <v>87</v>
       </c>
       <c r="H37" s="15"/>
-      <c r="J37" s="23" t="s">
-        <v>107</v>
-      </c>
-      <c r="K37" s="23" t="s">
-        <v>117</v>
-      </c>
-      <c r="L37" s="14">
-        <v>10</v>
-      </c>
+      <c r="J37" s="33" t="s">
+        <v>106</v>
+      </c>
+      <c r="K37" s="34" t="s">
+        <v>111</v>
+      </c>
+      <c r="L37" s="14"/>
     </row>
     <row r="38" spans="6:12" x14ac:dyDescent="0.25">
       <c r="J38" s="23" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="K38" s="23" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="L38" s="14">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="39" spans="6:12" x14ac:dyDescent="0.25">
       <c r="J39" s="23" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="K39" s="23" t="s">
         <v>118</v>
       </c>
       <c r="L39" s="14">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="40" spans="6:12" x14ac:dyDescent="0.25">
       <c r="J40" s="23" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="K40" s="23" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="L40" s="14">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="41" spans="6:12" x14ac:dyDescent="0.25">
       <c r="J41" s="23" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="K41" s="23" t="s">
+        <v>119</v>
+      </c>
+      <c r="L41" s="14">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="42" spans="6:12" x14ac:dyDescent="0.25">
+      <c r="J42" s="23" t="s">
+        <v>106</v>
+      </c>
+      <c r="K42" s="23" t="s">
+        <v>120</v>
+      </c>
+      <c r="L42" s="14">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="43" spans="6:12" ht="12" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J43" s="35" t="s">
+        <v>106</v>
+      </c>
+      <c r="K43" s="36" t="s">
         <v>121</v>
       </c>
-      <c r="L41" s="14">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="42" spans="6:12" ht="12" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="J42" s="46" t="s">
-        <v>107</v>
-      </c>
-      <c r="K42" s="47" t="s">
-        <v>122</v>
-      </c>
-      <c r="L42" s="15"/>
+      <c r="L43" s="15"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Changing Materials a bit
</commit_message>
<xml_diff>
--- a/Workshop_Materials.xlsx
+++ b/Workshop_Materials.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="149">
   <si>
     <t>List of Components</t>
   </si>
@@ -444,6 +444,24 @@
   </si>
   <si>
     <t>Decoupling Circuit</t>
+  </si>
+  <si>
+    <t>Titls</t>
+  </si>
+  <si>
+    <t>How to Read: Didoes</t>
+  </si>
+  <si>
+    <t>How to Read: Switches</t>
+  </si>
+  <si>
+    <t>How to Read: Relays</t>
+  </si>
+  <si>
+    <t>How to Read: Transistors</t>
+  </si>
+  <si>
+    <t>How to Read: PMIC</t>
   </si>
 </sst>
 </file>
@@ -925,7 +943,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1075,6 +1093,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1382,10 +1403,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:H62"/>
+  <dimension ref="B1:H65"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K17" sqref="K17"/>
+      <selection activeCell="K36" sqref="K36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="11.25" x14ac:dyDescent="0.25"/>
@@ -1747,7 +1768,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="20" spans="2:8" ht="12" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B20" s="14" t="s">
         <v>23</v>
       </c>
@@ -1755,13 +1776,13 @@
         <v>53</v>
       </c>
       <c r="D20" s="14"/>
-      <c r="F20" s="16" t="s">
+      <c r="F20" s="51" t="s">
         <v>56</v>
       </c>
-      <c r="G20" s="16" t="s">
-        <v>22</v>
-      </c>
-      <c r="H20" s="16" t="s">
+      <c r="G20" s="51" t="s">
+        <v>143</v>
+      </c>
+      <c r="H20" s="51" t="s">
         <v>55</v>
       </c>
     </row>
@@ -1775,15 +1796,13 @@
       <c r="D21" s="14">
         <v>11</v>
       </c>
-      <c r="F21" s="30" t="s">
-        <v>99</v>
-      </c>
-      <c r="G21" s="30" t="s">
-        <v>102</v>
-      </c>
-      <c r="H21" s="17">
-        <v>5</v>
-      </c>
+      <c r="F21" s="23" t="s">
+        <v>91</v>
+      </c>
+      <c r="G21" s="23" t="s">
+        <v>144</v>
+      </c>
+      <c r="H21" s="14"/>
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B22" s="14" t="s">
@@ -1794,14 +1813,12 @@
       </c>
       <c r="D22" s="14"/>
       <c r="F22" s="23" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="G22" s="23" t="s">
-        <v>103</v>
-      </c>
-      <c r="H22" s="14">
-        <v>5</v>
-      </c>
+        <v>145</v>
+      </c>
+      <c r="H22" s="14"/>
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B23" s="14" t="s">
@@ -1814,14 +1831,12 @@
         <v>4</v>
       </c>
       <c r="F23" s="23" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="G23" s="23" t="s">
-        <v>104</v>
-      </c>
-      <c r="H23" s="14">
-        <v>5</v>
-      </c>
+        <v>146</v>
+      </c>
+      <c r="H23" s="14"/>
     </row>
     <row r="24" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B24" s="14" t="s">
@@ -1834,14 +1849,12 @@
         <v>12</v>
       </c>
       <c r="F24" s="23" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="G24" s="23" t="s">
-        <v>100</v>
-      </c>
-      <c r="H24" s="14">
-        <v>5</v>
-      </c>
+        <v>147</v>
+      </c>
+      <c r="H24" s="14"/>
     </row>
     <row r="25" spans="2:8" ht="12" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B25" s="15" t="s">
@@ -1853,27 +1866,15 @@
       <c r="D25" s="15">
         <v>13</v>
       </c>
-      <c r="F25" s="23" t="s">
-        <v>99</v>
-      </c>
-      <c r="G25" s="23" t="s">
-        <v>136</v>
-      </c>
-      <c r="H25" s="14">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="26" spans="2:8" ht="12" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F26" s="25" t="s">
-        <v>99</v>
-      </c>
-      <c r="G26" s="25" t="s">
-        <v>105</v>
-      </c>
-      <c r="H26" s="15">
-        <v>6</v>
-      </c>
-    </row>
+      <c r="F25" s="25" t="s">
+        <v>91</v>
+      </c>
+      <c r="G25" s="25" t="s">
+        <v>148</v>
+      </c>
+      <c r="H25" s="15"/>
+    </row>
+    <row r="26" spans="2:8" ht="12" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="27" spans="2:8" ht="12" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B27" s="16" t="s">
         <v>56</v>
@@ -1884,8 +1885,17 @@
       <c r="D27" s="16" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="28" spans="2:8" ht="12" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F27" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="G27" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="H27" s="16" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="28" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B28" s="13" t="s">
         <v>24</v>
       </c>
@@ -1895,14 +1905,14 @@
       <c r="D28" s="13">
         <v>0</v>
       </c>
-      <c r="F28" s="16" t="s">
-        <v>56</v>
-      </c>
-      <c r="G28" s="16" t="s">
-        <v>22</v>
-      </c>
-      <c r="H28" s="16" t="s">
-        <v>55</v>
+      <c r="F28" s="30" t="s">
+        <v>99</v>
+      </c>
+      <c r="G28" s="30" t="s">
+        <v>102</v>
+      </c>
+      <c r="H28" s="17">
+        <v>5</v>
       </c>
     </row>
     <row r="29" spans="2:8" x14ac:dyDescent="0.25">
@@ -1915,14 +1925,14 @@
       <c r="D29" s="14">
         <v>1</v>
       </c>
-      <c r="F29" s="30" t="s">
-        <v>106</v>
-      </c>
-      <c r="G29" s="30" t="s">
-        <v>112</v>
-      </c>
-      <c r="H29" s="30" t="s">
-        <v>141</v>
+      <c r="F29" s="23" t="s">
+        <v>99</v>
+      </c>
+      <c r="G29" s="23" t="s">
+        <v>103</v>
+      </c>
+      <c r="H29" s="14">
+        <v>5</v>
       </c>
     </row>
     <row r="30" spans="2:8" x14ac:dyDescent="0.25">
@@ -1936,13 +1946,13 @@
         <v>2</v>
       </c>
       <c r="F30" s="23" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="G30" s="23" t="s">
-        <v>115</v>
-      </c>
-      <c r="H30" s="23" t="s">
-        <v>141</v>
+        <v>104</v>
+      </c>
+      <c r="H30" s="14">
+        <v>5</v>
       </c>
     </row>
     <row r="31" spans="2:8" x14ac:dyDescent="0.25">
@@ -1956,13 +1966,13 @@
         <v>3</v>
       </c>
       <c r="F31" s="23" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="G31" s="23" t="s">
-        <v>113</v>
-      </c>
-      <c r="H31" s="23" t="s">
-        <v>141</v>
+        <v>100</v>
+      </c>
+      <c r="H31" s="14">
+        <v>5</v>
       </c>
     </row>
     <row r="32" spans="2:8" x14ac:dyDescent="0.25">
@@ -1976,16 +1986,16 @@
         <v>4</v>
       </c>
       <c r="F32" s="23" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="G32" s="23" t="s">
-        <v>114</v>
-      </c>
-      <c r="H32" s="23" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="33" spans="2:8" x14ac:dyDescent="0.25">
+        <v>136</v>
+      </c>
+      <c r="H32" s="14">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="33" spans="2:8" ht="12" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B33" s="14" t="s">
         <v>24</v>
       </c>
@@ -1993,17 +2003,17 @@
         <v>59</v>
       </c>
       <c r="D33" s="14"/>
-      <c r="F33" s="23" t="s">
-        <v>106</v>
-      </c>
-      <c r="G33" s="23" t="s">
-        <v>142</v>
-      </c>
-      <c r="H33" s="23" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="34" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="F33" s="25" t="s">
+        <v>99</v>
+      </c>
+      <c r="G33" s="25" t="s">
+        <v>105</v>
+      </c>
+      <c r="H33" s="15">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="34" spans="2:8" ht="12" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B34" s="14" t="s">
         <v>24</v>
       </c>
@@ -2013,15 +2023,8 @@
       <c r="D34" s="14">
         <v>5</v>
       </c>
-      <c r="F34" s="33" t="s">
-        <v>106</v>
-      </c>
-      <c r="G34" s="34" t="s">
-        <v>109</v>
-      </c>
-      <c r="H34" s="14"/>
-    </row>
-    <row r="35" spans="2:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="35" spans="2:8" ht="12" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B35" s="14" t="s">
         <v>24</v>
       </c>
@@ -2031,14 +2034,14 @@
       <c r="D35" s="14">
         <v>6</v>
       </c>
-      <c r="F35" s="23" t="s">
-        <v>106</v>
-      </c>
-      <c r="G35" s="23" t="s">
-        <v>110</v>
-      </c>
-      <c r="H35" s="23">
-        <v>8</v>
+      <c r="F35" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="G35" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="H35" s="16" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="36" spans="2:8" x14ac:dyDescent="0.25">
@@ -2049,14 +2052,14 @@
         <v>66</v>
       </c>
       <c r="D36" s="14"/>
-      <c r="F36" s="23" t="s">
+      <c r="F36" s="30" t="s">
         <v>106</v>
       </c>
-      <c r="G36" s="23" t="s">
-        <v>110</v>
-      </c>
-      <c r="H36" s="23">
-        <v>8</v>
+      <c r="G36" s="30" t="s">
+        <v>112</v>
+      </c>
+      <c r="H36" s="30" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="37" spans="2:8" x14ac:dyDescent="0.25">
@@ -2073,10 +2076,10 @@
         <v>106</v>
       </c>
       <c r="G37" s="23" t="s">
-        <v>139</v>
+        <v>115</v>
       </c>
       <c r="H37" s="23" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
     </row>
     <row r="38" spans="2:8" x14ac:dyDescent="0.25">
@@ -2093,10 +2096,10 @@
         <v>106</v>
       </c>
       <c r="G38" s="23" t="s">
-        <v>140</v>
+        <v>113</v>
       </c>
       <c r="H38" s="23" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
     </row>
     <row r="39" spans="2:8" x14ac:dyDescent="0.25">
@@ -2107,13 +2110,15 @@
         <v>67</v>
       </c>
       <c r="D39" s="14"/>
-      <c r="F39" s="33" t="s">
+      <c r="F39" s="23" t="s">
         <v>106</v>
       </c>
-      <c r="G39" s="34" t="s">
-        <v>111</v>
-      </c>
-      <c r="H39" s="14"/>
+      <c r="G39" s="23" t="s">
+        <v>114</v>
+      </c>
+      <c r="H39" s="23" t="s">
+        <v>141</v>
+      </c>
     </row>
     <row r="40" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B40" s="14" t="s">
@@ -2129,10 +2134,10 @@
         <v>106</v>
       </c>
       <c r="G40" s="23" t="s">
-        <v>116</v>
-      </c>
-      <c r="H40" s="14">
-        <v>9</v>
+        <v>142</v>
+      </c>
+      <c r="H40" s="23" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="41" spans="2:8" x14ac:dyDescent="0.25">
@@ -2145,15 +2150,13 @@
       <c r="D41" s="14" t="s">
         <v>76</v>
       </c>
-      <c r="F41" s="23" t="s">
+      <c r="F41" s="33" t="s">
         <v>106</v>
       </c>
-      <c r="G41" s="23" t="s">
-        <v>118</v>
-      </c>
-      <c r="H41" s="14">
-        <v>9</v>
-      </c>
+      <c r="G41" s="34" t="s">
+        <v>109</v>
+      </c>
+      <c r="H41" s="14"/>
     </row>
     <row r="42" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B42" s="14" t="s">
@@ -2169,10 +2172,10 @@
         <v>106</v>
       </c>
       <c r="G42" s="23" t="s">
-        <v>117</v>
-      </c>
-      <c r="H42" s="14">
-        <v>9</v>
+        <v>110</v>
+      </c>
+      <c r="H42" s="23">
+        <v>8</v>
       </c>
     </row>
     <row r="43" spans="2:8" x14ac:dyDescent="0.25">
@@ -2189,10 +2192,10 @@
         <v>106</v>
       </c>
       <c r="G43" s="23" t="s">
-        <v>119</v>
-      </c>
-      <c r="H43" s="14">
-        <v>9</v>
+        <v>110</v>
+      </c>
+      <c r="H43" s="23">
+        <v>8</v>
       </c>
     </row>
     <row r="44" spans="2:8" x14ac:dyDescent="0.25">
@@ -2209,13 +2212,13 @@
         <v>106</v>
       </c>
       <c r="G44" s="23" t="s">
-        <v>120</v>
-      </c>
-      <c r="H44" s="14">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="45" spans="2:8" ht="12" thickBot="1" x14ac:dyDescent="0.3">
+        <v>139</v>
+      </c>
+      <c r="H44" s="23" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="45" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B45" s="14" t="s">
         <v>24</v>
       </c>
@@ -2225,15 +2228,17 @@
       <c r="D45" s="14">
         <v>12</v>
       </c>
-      <c r="F45" s="35" t="s">
+      <c r="F45" s="23" t="s">
         <v>106</v>
       </c>
-      <c r="G45" s="36" t="s">
-        <v>121</v>
-      </c>
-      <c r="H45" s="15"/>
-    </row>
-    <row r="46" spans="2:8" ht="12" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G45" s="23" t="s">
+        <v>140</v>
+      </c>
+      <c r="H45" s="23" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="46" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B46" s="14" t="s">
         <v>24</v>
       </c>
@@ -2243,8 +2248,15 @@
       <c r="D46" s="14">
         <v>13</v>
       </c>
-    </row>
-    <row r="47" spans="2:8" ht="12" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F46" s="33" t="s">
+        <v>106</v>
+      </c>
+      <c r="G46" s="34" t="s">
+        <v>111</v>
+      </c>
+      <c r="H46" s="14"/>
+    </row>
+    <row r="47" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B47" s="14" t="s">
         <v>24</v>
       </c>
@@ -2254,14 +2266,14 @@
       <c r="D47" s="14">
         <v>14</v>
       </c>
-      <c r="F47" s="16" t="s">
-        <v>56</v>
-      </c>
-      <c r="G47" s="16" t="s">
-        <v>22</v>
-      </c>
-      <c r="H47" s="16" t="s">
-        <v>55</v>
+      <c r="F47" s="23" t="s">
+        <v>106</v>
+      </c>
+      <c r="G47" s="23" t="s">
+        <v>116</v>
+      </c>
+      <c r="H47" s="14">
+        <v>9</v>
       </c>
     </row>
     <row r="48" spans="2:8" x14ac:dyDescent="0.25">
@@ -2274,14 +2286,14 @@
       <c r="D48" s="14">
         <v>15</v>
       </c>
-      <c r="F48" s="30" t="s">
-        <v>122</v>
-      </c>
-      <c r="G48" s="30" t="s">
-        <v>123</v>
-      </c>
-      <c r="H48" s="17">
-        <v>10</v>
+      <c r="F48" s="23" t="s">
+        <v>106</v>
+      </c>
+      <c r="G48" s="23" t="s">
+        <v>118</v>
+      </c>
+      <c r="H48" s="14">
+        <v>9</v>
       </c>
     </row>
     <row r="49" spans="2:8" x14ac:dyDescent="0.25">
@@ -2295,13 +2307,13 @@
         <v>86</v>
       </c>
       <c r="F49" s="23" t="s">
-        <v>122</v>
+        <v>106</v>
       </c>
       <c r="G49" s="23" t="s">
-        <v>129</v>
+        <v>117</v>
       </c>
       <c r="H49" s="14">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="50" spans="2:8" x14ac:dyDescent="0.25">
@@ -2315,13 +2327,13 @@
         <v>85</v>
       </c>
       <c r="F50" s="23" t="s">
-        <v>122</v>
+        <v>106</v>
       </c>
       <c r="G50" s="23" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="H50" s="14">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="51" spans="2:8" x14ac:dyDescent="0.25">
@@ -2333,16 +2345,16 @@
       </c>
       <c r="D51" s="14"/>
       <c r="F51" s="23" t="s">
-        <v>122</v>
+        <v>106</v>
       </c>
       <c r="G51" s="23" t="s">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="H51" s="14">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="52" spans="2:8" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="52" spans="2:8" ht="12" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B52" s="14" t="s">
         <v>24</v>
       </c>
@@ -2352,17 +2364,15 @@
       <c r="D52" s="14">
         <v>22</v>
       </c>
-      <c r="F52" s="23" t="s">
-        <v>122</v>
-      </c>
-      <c r="G52" s="23" t="s">
-        <v>132</v>
-      </c>
-      <c r="H52" s="14">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="53" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="F52" s="35" t="s">
+        <v>106</v>
+      </c>
+      <c r="G52" s="36" t="s">
+        <v>121</v>
+      </c>
+      <c r="H52" s="15"/>
+    </row>
+    <row r="53" spans="2:8" ht="12" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B53" s="14" t="s">
         <v>24</v>
       </c>
@@ -2372,17 +2382,8 @@
       <c r="D53" s="14">
         <v>23</v>
       </c>
-      <c r="F53" s="23" t="s">
-        <v>122</v>
-      </c>
-      <c r="G53" s="23" t="s">
-        <v>131</v>
-      </c>
-      <c r="H53" s="14">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="54" spans="2:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="54" spans="2:8" ht="12" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B54" s="14" t="s">
         <v>24</v>
       </c>
@@ -2392,17 +2393,17 @@
       <c r="D54" s="14">
         <v>9</v>
       </c>
-      <c r="F54" s="23" t="s">
-        <v>122</v>
-      </c>
-      <c r="G54" s="23" t="s">
-        <v>133</v>
-      </c>
-      <c r="H54" s="14">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="55" spans="2:8" ht="12" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F54" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="G54" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="H54" s="16" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="55" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B55" s="14" t="s">
         <v>24</v>
       </c>
@@ -2412,15 +2413,17 @@
       <c r="D55" s="14">
         <v>10</v>
       </c>
-      <c r="F55" s="35" t="s">
+      <c r="F55" s="30" t="s">
         <v>122</v>
       </c>
-      <c r="G55" s="36" t="s">
-        <v>121</v>
-      </c>
-      <c r="H55" s="15"/>
-    </row>
-    <row r="56" spans="2:8" ht="12" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G55" s="30" t="s">
+        <v>123</v>
+      </c>
+      <c r="H55" s="17">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="56" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B56" s="14" t="s">
         <v>24</v>
       </c>
@@ -2430,8 +2433,17 @@
       <c r="D56" s="14">
         <v>11</v>
       </c>
-    </row>
-    <row r="57" spans="2:8" ht="12" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F56" s="23" t="s">
+        <v>122</v>
+      </c>
+      <c r="G56" s="23" t="s">
+        <v>129</v>
+      </c>
+      <c r="H56" s="14">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="57" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B57" s="14" t="s">
         <v>24</v>
       </c>
@@ -2439,17 +2451,17 @@
         <v>81</v>
       </c>
       <c r="D57" s="14"/>
-      <c r="F57" s="27" t="s">
-        <v>56</v>
-      </c>
-      <c r="G57" s="28" t="s">
-        <v>22</v>
-      </c>
-      <c r="H57" s="29" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="58" spans="2:8" ht="12" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F57" s="23" t="s">
+        <v>122</v>
+      </c>
+      <c r="G57" s="23" t="s">
+        <v>114</v>
+      </c>
+      <c r="H57" s="14">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="58" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B58" s="14" t="s">
         <v>24</v>
       </c>
@@ -2459,13 +2471,15 @@
       <c r="D58" s="14">
         <v>19</v>
       </c>
-      <c r="F58" s="37" t="s">
-        <v>134</v>
-      </c>
-      <c r="G58" s="38" t="s">
-        <v>135</v>
-      </c>
-      <c r="H58" s="39"/>
+      <c r="F58" s="23" t="s">
+        <v>122</v>
+      </c>
+      <c r="G58" s="23" t="s">
+        <v>130</v>
+      </c>
+      <c r="H58" s="14">
+        <v>10</v>
+      </c>
     </row>
     <row r="59" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B59" s="14" t="s">
@@ -2477,6 +2491,15 @@
       <c r="D59" s="23" t="s">
         <v>89</v>
       </c>
+      <c r="F59" s="23" t="s">
+        <v>122</v>
+      </c>
+      <c r="G59" s="23" t="s">
+        <v>132</v>
+      </c>
+      <c r="H59" s="14">
+        <v>10</v>
+      </c>
     </row>
     <row r="60" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B60" s="14" t="s">
@@ -2488,6 +2511,15 @@
       <c r="D60" s="23" t="s">
         <v>90</v>
       </c>
+      <c r="F60" s="23" t="s">
+        <v>122</v>
+      </c>
+      <c r="G60" s="23" t="s">
+        <v>131</v>
+      </c>
+      <c r="H60" s="14">
+        <v>10</v>
+      </c>
     </row>
     <row r="61" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B61" s="14" t="s">
@@ -2499,6 +2531,15 @@
       <c r="D61" s="14">
         <v>21</v>
       </c>
+      <c r="F61" s="23" t="s">
+        <v>122</v>
+      </c>
+      <c r="G61" s="23" t="s">
+        <v>133</v>
+      </c>
+      <c r="H61" s="14">
+        <v>10</v>
+      </c>
     </row>
     <row r="62" spans="2:8" ht="12" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B62" s="25" t="s">
@@ -2508,6 +2549,34 @@
         <v>87</v>
       </c>
       <c r="D62" s="15"/>
+      <c r="F62" s="35" t="s">
+        <v>122</v>
+      </c>
+      <c r="G62" s="36" t="s">
+        <v>121</v>
+      </c>
+      <c r="H62" s="15"/>
+    </row>
+    <row r="63" spans="2:8" ht="12" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="64" spans="2:8" ht="12" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F64" s="27" t="s">
+        <v>56</v>
+      </c>
+      <c r="G64" s="28" t="s">
+        <v>22</v>
+      </c>
+      <c r="H64" s="29" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="65" spans="6:8" ht="12" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F65" s="37" t="s">
+        <v>134</v>
+      </c>
+      <c r="G65" s="38" t="s">
+        <v>135</v>
+      </c>
+      <c r="H65" s="39"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Adding 5th Slide for Eagle CAD
</commit_message>
<xml_diff>
--- a/Workshop_Materials.xlsx
+++ b/Workshop_Materials.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="150">
   <si>
     <t>List of Components</t>
   </si>
@@ -462,6 +462,9 @@
   </si>
   <si>
     <t>How to Read: PMIC</t>
+  </si>
+  <si>
+    <t>How to Read: Microcontrollers</t>
   </si>
 </sst>
 </file>
@@ -1403,10 +1406,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:H65"/>
+  <dimension ref="B1:H66"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K29" sqref="K29"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="L27" sqref="L27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="11.25" x14ac:dyDescent="0.25"/>
@@ -1834,7 +1837,7 @@
         <v>91</v>
       </c>
       <c r="G23" s="23" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="H23" s="14"/>
     </row>
@@ -1852,7 +1855,7 @@
         <v>91</v>
       </c>
       <c r="G24" s="23" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="H24" s="14"/>
     </row>
@@ -1866,15 +1869,23 @@
       <c r="D25" s="15">
         <v>13</v>
       </c>
-      <c r="F25" s="25" t="s">
+      <c r="F25" s="23" t="s">
         <v>91</v>
       </c>
-      <c r="G25" s="25" t="s">
+      <c r="G25" s="23" t="s">
+        <v>147</v>
+      </c>
+      <c r="H25" s="14"/>
+    </row>
+    <row r="26" spans="2:8" ht="12" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F26" s="25" t="s">
+        <v>91</v>
+      </c>
+      <c r="G26" s="25" t="s">
         <v>148</v>
       </c>
-      <c r="H25" s="15"/>
-    </row>
-    <row r="26" spans="2:8" ht="12" thickBot="1" x14ac:dyDescent="0.3"/>
+      <c r="H26" s="15"/>
+    </row>
     <row r="27" spans="2:8" ht="12" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B27" s="16" t="s">
         <v>56</v>
@@ -1885,17 +1896,8 @@
       <c r="D27" s="16" t="s">
         <v>55</v>
       </c>
-      <c r="F27" s="16" t="s">
-        <v>56</v>
-      </c>
-      <c r="G27" s="16" t="s">
-        <v>22</v>
-      </c>
-      <c r="H27" s="16" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="28" spans="2:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="28" spans="2:8" ht="12" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B28" s="13" t="s">
         <v>24</v>
       </c>
@@ -1905,14 +1907,14 @@
       <c r="D28" s="13">
         <v>0</v>
       </c>
-      <c r="F28" s="30" t="s">
-        <v>99</v>
-      </c>
-      <c r="G28" s="30" t="s">
-        <v>102</v>
-      </c>
-      <c r="H28" s="17">
-        <v>5</v>
+      <c r="F28" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="G28" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="H28" s="16" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="29" spans="2:8" x14ac:dyDescent="0.25">
@@ -1925,13 +1927,13 @@
       <c r="D29" s="14">
         <v>1</v>
       </c>
-      <c r="F29" s="23" t="s">
+      <c r="F29" s="30" t="s">
         <v>99</v>
       </c>
-      <c r="G29" s="23" t="s">
-        <v>103</v>
-      </c>
-      <c r="H29" s="14">
+      <c r="G29" s="30" t="s">
+        <v>102</v>
+      </c>
+      <c r="H29" s="17">
         <v>5</v>
       </c>
     </row>
@@ -1949,7 +1951,7 @@
         <v>99</v>
       </c>
       <c r="G30" s="23" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H30" s="14">
         <v>5</v>
@@ -1969,7 +1971,7 @@
         <v>99</v>
       </c>
       <c r="G31" s="23" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="H31" s="14">
         <v>5</v>
@@ -1989,13 +1991,13 @@
         <v>99</v>
       </c>
       <c r="G32" s="23" t="s">
-        <v>136</v>
+        <v>100</v>
       </c>
       <c r="H32" s="14">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="33" spans="2:8" ht="12" thickBot="1" x14ac:dyDescent="0.3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="33" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B33" s="14" t="s">
         <v>24</v>
       </c>
@@ -2003,13 +2005,13 @@
         <v>59</v>
       </c>
       <c r="D33" s="14"/>
-      <c r="F33" s="25" t="s">
+      <c r="F33" s="23" t="s">
         <v>99</v>
       </c>
-      <c r="G33" s="25" t="s">
-        <v>105</v>
-      </c>
-      <c r="H33" s="15">
+      <c r="G33" s="23" t="s">
+        <v>136</v>
+      </c>
+      <c r="H33" s="14">
         <v>6</v>
       </c>
     </row>
@@ -2023,6 +2025,15 @@
       <c r="D34" s="14">
         <v>5</v>
       </c>
+      <c r="F34" s="25" t="s">
+        <v>99</v>
+      </c>
+      <c r="G34" s="25" t="s">
+        <v>105</v>
+      </c>
+      <c r="H34" s="15">
+        <v>6</v>
+      </c>
     </row>
     <row r="35" spans="2:8" ht="12" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B35" s="14" t="s">
@@ -2034,17 +2045,8 @@
       <c r="D35" s="14">
         <v>6</v>
       </c>
-      <c r="F35" s="16" t="s">
-        <v>56</v>
-      </c>
-      <c r="G35" s="16" t="s">
-        <v>22</v>
-      </c>
-      <c r="H35" s="16" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="36" spans="2:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="36" spans="2:8" ht="12" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B36" s="14" t="s">
         <v>24</v>
       </c>
@@ -2052,14 +2054,14 @@
         <v>66</v>
       </c>
       <c r="D36" s="14"/>
-      <c r="F36" s="30" t="s">
-        <v>106</v>
-      </c>
-      <c r="G36" s="30" t="s">
-        <v>112</v>
-      </c>
-      <c r="H36" s="30" t="s">
-        <v>141</v>
+      <c r="F36" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="G36" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="H36" s="16" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="37" spans="2:8" x14ac:dyDescent="0.25">
@@ -2072,13 +2074,13 @@
       <c r="D37" s="14">
         <v>7</v>
       </c>
-      <c r="F37" s="23" t="s">
+      <c r="F37" s="30" t="s">
         <v>106</v>
       </c>
-      <c r="G37" s="23" t="s">
-        <v>115</v>
-      </c>
-      <c r="H37" s="23" t="s">
+      <c r="G37" s="30" t="s">
+        <v>112</v>
+      </c>
+      <c r="H37" s="30" t="s">
         <v>141</v>
       </c>
     </row>
@@ -2096,7 +2098,7 @@
         <v>106</v>
       </c>
       <c r="G38" s="23" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="H38" s="23" t="s">
         <v>141</v>
@@ -2114,7 +2116,7 @@
         <v>106</v>
       </c>
       <c r="G39" s="23" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="H39" s="23" t="s">
         <v>141</v>
@@ -2134,7 +2136,7 @@
         <v>106</v>
       </c>
       <c r="G40" s="23" t="s">
-        <v>142</v>
+        <v>114</v>
       </c>
       <c r="H40" s="23" t="s">
         <v>141</v>
@@ -2150,13 +2152,15 @@
       <c r="D41" s="14" t="s">
         <v>76</v>
       </c>
-      <c r="F41" s="33" t="s">
+      <c r="F41" s="23" t="s">
         <v>106</v>
       </c>
-      <c r="G41" s="34" t="s">
-        <v>109</v>
-      </c>
-      <c r="H41" s="14"/>
+      <c r="G41" s="23" t="s">
+        <v>142</v>
+      </c>
+      <c r="H41" s="23" t="s">
+        <v>141</v>
+      </c>
     </row>
     <row r="42" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B42" s="14" t="s">
@@ -2168,15 +2172,13 @@
       <c r="D42" s="14" t="s">
         <v>82</v>
       </c>
-      <c r="F42" s="23" t="s">
+      <c r="F42" s="33" t="s">
         <v>106</v>
       </c>
-      <c r="G42" s="23" t="s">
-        <v>110</v>
-      </c>
-      <c r="H42" s="23">
-        <v>8</v>
-      </c>
+      <c r="G42" s="34" t="s">
+        <v>109</v>
+      </c>
+      <c r="H42" s="14"/>
     </row>
     <row r="43" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B43" s="14" t="s">
@@ -2212,10 +2214,10 @@
         <v>106</v>
       </c>
       <c r="G44" s="23" t="s">
-        <v>139</v>
-      </c>
-      <c r="H44" s="23" t="s">
-        <v>138</v>
+        <v>110</v>
+      </c>
+      <c r="H44" s="23">
+        <v>8</v>
       </c>
     </row>
     <row r="45" spans="2:8" x14ac:dyDescent="0.25">
@@ -2232,7 +2234,7 @@
         <v>106</v>
       </c>
       <c r="G45" s="23" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="H45" s="23" t="s">
         <v>138</v>
@@ -2248,13 +2250,15 @@
       <c r="D46" s="14">
         <v>13</v>
       </c>
-      <c r="F46" s="33" t="s">
+      <c r="F46" s="23" t="s">
         <v>106</v>
       </c>
-      <c r="G46" s="34" t="s">
-        <v>111</v>
-      </c>
-      <c r="H46" s="14"/>
+      <c r="G46" s="23" t="s">
+        <v>140</v>
+      </c>
+      <c r="H46" s="23" t="s">
+        <v>138</v>
+      </c>
     </row>
     <row r="47" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B47" s="14" t="s">
@@ -2266,15 +2270,13 @@
       <c r="D47" s="14">
         <v>14</v>
       </c>
-      <c r="F47" s="23" t="s">
+      <c r="F47" s="33" t="s">
         <v>106</v>
       </c>
-      <c r="G47" s="23" t="s">
-        <v>116</v>
-      </c>
-      <c r="H47" s="14">
-        <v>9</v>
-      </c>
+      <c r="G47" s="34" t="s">
+        <v>111</v>
+      </c>
+      <c r="H47" s="14"/>
     </row>
     <row r="48" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B48" s="14" t="s">
@@ -2290,7 +2292,7 @@
         <v>106</v>
       </c>
       <c r="G48" s="23" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="H48" s="14">
         <v>9</v>
@@ -2310,7 +2312,7 @@
         <v>106</v>
       </c>
       <c r="G49" s="23" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="H49" s="14">
         <v>9</v>
@@ -2330,7 +2332,7 @@
         <v>106</v>
       </c>
       <c r="G50" s="23" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="H50" s="14">
         <v>9</v>
@@ -2348,13 +2350,13 @@
         <v>106</v>
       </c>
       <c r="G51" s="23" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="H51" s="14">
         <v>9</v>
       </c>
     </row>
-    <row r="52" spans="2:8" ht="12" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B52" s="14" t="s">
         <v>24</v>
       </c>
@@ -2364,13 +2366,15 @@
       <c r="D52" s="14">
         <v>22</v>
       </c>
-      <c r="F52" s="35" t="s">
+      <c r="F52" s="23" t="s">
         <v>106</v>
       </c>
-      <c r="G52" s="36" t="s">
-        <v>121</v>
-      </c>
-      <c r="H52" s="15"/>
+      <c r="G52" s="23" t="s">
+        <v>120</v>
+      </c>
+      <c r="H52" s="14">
+        <v>9</v>
+      </c>
     </row>
     <row r="53" spans="2:8" ht="12" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B53" s="14" t="s">
@@ -2382,6 +2386,13 @@
       <c r="D53" s="14">
         <v>23</v>
       </c>
+      <c r="F53" s="35" t="s">
+        <v>106</v>
+      </c>
+      <c r="G53" s="36" t="s">
+        <v>121</v>
+      </c>
+      <c r="H53" s="15"/>
     </row>
     <row r="54" spans="2:8" ht="12" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B54" s="14" t="s">
@@ -2393,17 +2404,8 @@
       <c r="D54" s="14">
         <v>9</v>
       </c>
-      <c r="F54" s="16" t="s">
-        <v>56</v>
-      </c>
-      <c r="G54" s="16" t="s">
-        <v>22</v>
-      </c>
-      <c r="H54" s="16" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="55" spans="2:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="55" spans="2:8" ht="12" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B55" s="14" t="s">
         <v>24</v>
       </c>
@@ -2413,14 +2415,14 @@
       <c r="D55" s="14">
         <v>10</v>
       </c>
-      <c r="F55" s="30" t="s">
-        <v>122</v>
-      </c>
-      <c r="G55" s="30" t="s">
-        <v>123</v>
-      </c>
-      <c r="H55" s="17">
-        <v>10</v>
+      <c r="F55" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="G55" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="H55" s="16" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="56" spans="2:8" x14ac:dyDescent="0.25">
@@ -2433,13 +2435,13 @@
       <c r="D56" s="14">
         <v>11</v>
       </c>
-      <c r="F56" s="23" t="s">
+      <c r="F56" s="30" t="s">
         <v>122</v>
       </c>
-      <c r="G56" s="23" t="s">
-        <v>129</v>
-      </c>
-      <c r="H56" s="14">
+      <c r="G56" s="30" t="s">
+        <v>123</v>
+      </c>
+      <c r="H56" s="17">
         <v>10</v>
       </c>
     </row>
@@ -2455,7 +2457,7 @@
         <v>122</v>
       </c>
       <c r="G57" s="23" t="s">
-        <v>114</v>
+        <v>129</v>
       </c>
       <c r="H57" s="14">
         <v>10</v>
@@ -2475,7 +2477,7 @@
         <v>122</v>
       </c>
       <c r="G58" s="23" t="s">
-        <v>130</v>
+        <v>114</v>
       </c>
       <c r="H58" s="14">
         <v>10</v>
@@ -2495,7 +2497,7 @@
         <v>122</v>
       </c>
       <c r="G59" s="23" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="H59" s="14">
         <v>10</v>
@@ -2515,7 +2517,7 @@
         <v>122</v>
       </c>
       <c r="G60" s="23" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="H60" s="14">
         <v>10</v>
@@ -2535,7 +2537,7 @@
         <v>122</v>
       </c>
       <c r="G61" s="23" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="H61" s="14">
         <v>10</v>
@@ -2549,34 +2551,45 @@
         <v>87</v>
       </c>
       <c r="D62" s="15"/>
-      <c r="F62" s="35" t="s">
+      <c r="F62" s="23" t="s">
         <v>122</v>
       </c>
-      <c r="G62" s="36" t="s">
+      <c r="G62" s="23" t="s">
+        <v>133</v>
+      </c>
+      <c r="H62" s="14">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="63" spans="2:8" ht="12" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F63" s="35" t="s">
+        <v>122</v>
+      </c>
+      <c r="G63" s="36" t="s">
         <v>121</v>
       </c>
-      <c r="H62" s="15"/>
-    </row>
-    <row r="63" spans="2:8" ht="12" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="64" spans="2:8" ht="12" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F64" s="27" t="s">
+      <c r="H63" s="15"/>
+    </row>
+    <row r="64" spans="2:8" ht="12" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="65" spans="6:8" ht="12" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F65" s="27" t="s">
         <v>56</v>
       </c>
-      <c r="G64" s="28" t="s">
+      <c r="G65" s="28" t="s">
         <v>22</v>
       </c>
-      <c r="H64" s="29" t="s">
+      <c r="H65" s="29" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="65" spans="6:8" ht="12" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F65" s="37" t="s">
+    <row r="66" spans="6:8" ht="12" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F66" s="37" t="s">
         <v>134</v>
       </c>
-      <c r="G65" s="38" t="s">
+      <c r="G66" s="38" t="s">
         <v>135</v>
       </c>
-      <c r="H65" s="39"/>
+      <c r="H66" s="39"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added Workshop Slide #7
</commit_message>
<xml_diff>
--- a/Workshop_Materials.xlsx
+++ b/Workshop_Materials.xlsx
@@ -1126,6 +1126,30 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1157,30 +1181,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1490,8 +1490,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:H66"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K15" sqref="K15"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="K39" sqref="K39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="11.25" x14ac:dyDescent="0.25"/>
@@ -1861,13 +1861,13 @@
         <v>53</v>
       </c>
       <c r="D20" s="14"/>
-      <c r="F20" s="57" t="s">
+      <c r="F20" s="46" t="s">
         <v>56</v>
       </c>
       <c r="G20" s="16" t="s">
         <v>143</v>
       </c>
-      <c r="H20" s="58" t="s">
+      <c r="H20" s="47" t="s">
         <v>55</v>
       </c>
     </row>
@@ -1881,13 +1881,13 @@
       <c r="D21" s="14">
         <v>11</v>
       </c>
-      <c r="F21" s="55" t="s">
+      <c r="F21" s="44" t="s">
         <v>91</v>
       </c>
       <c r="G21" s="30" t="s">
         <v>144</v>
       </c>
-      <c r="H21" s="56"/>
+      <c r="H21" s="45"/>
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B22" s="14" t="s">
@@ -1897,13 +1897,13 @@
         <v>54</v>
       </c>
       <c r="D22" s="14"/>
-      <c r="F22" s="51" t="s">
+      <c r="F22" s="40" t="s">
         <v>91</v>
       </c>
       <c r="G22" s="23" t="s">
         <v>149</v>
       </c>
-      <c r="H22" s="53"/>
+      <c r="H22" s="42"/>
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B23" s="14" t="s">
@@ -1915,13 +1915,13 @@
       <c r="D23" s="14">
         <v>4</v>
       </c>
-      <c r="F23" s="51" t="s">
+      <c r="F23" s="40" t="s">
         <v>91</v>
       </c>
       <c r="G23" s="23" t="s">
         <v>145</v>
       </c>
-      <c r="H23" s="53"/>
+      <c r="H23" s="42"/>
     </row>
     <row r="24" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B24" s="14" t="s">
@@ -1933,13 +1933,13 @@
       <c r="D24" s="14">
         <v>12</v>
       </c>
-      <c r="F24" s="51" t="s">
+      <c r="F24" s="40" t="s">
         <v>91</v>
       </c>
       <c r="G24" s="23" t="s">
         <v>146</v>
       </c>
-      <c r="H24" s="53"/>
+      <c r="H24" s="42"/>
     </row>
     <row r="25" spans="2:8" ht="12" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B25" s="15" t="s">
@@ -1951,22 +1951,22 @@
       <c r="D25" s="15">
         <v>13</v>
       </c>
-      <c r="F25" s="51" t="s">
+      <c r="F25" s="40" t="s">
         <v>91</v>
       </c>
       <c r="G25" s="23" t="s">
         <v>147</v>
       </c>
-      <c r="H25" s="53"/>
+      <c r="H25" s="42"/>
     </row>
     <row r="26" spans="2:8" ht="12" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F26" s="52" t="s">
+      <c r="F26" s="41" t="s">
         <v>91</v>
       </c>
       <c r="G26" s="25" t="s">
         <v>148</v>
       </c>
-      <c r="H26" s="54"/>
+      <c r="H26" s="43"/>
     </row>
     <row r="27" spans="2:8" ht="12" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B27" s="16" t="s">
@@ -2700,13 +2700,13 @@
   <sheetData>
     <row r="1" spans="2:6" ht="11.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="2" spans="2:6" ht="11.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="40" t="s">
+      <c r="B2" s="48" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="41"/>
-      <c r="D2" s="41"/>
-      <c r="E2" s="41"/>
-      <c r="F2" s="42"/>
+      <c r="C2" s="49"/>
+      <c r="D2" s="49"/>
+      <c r="E2" s="49"/>
+      <c r="F2" s="50"/>
     </row>
     <row r="3" spans="2:6" ht="11.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B3" s="9" t="s">
@@ -2996,11 +2996,11 @@
       </c>
     </row>
     <row r="19" spans="2:6" ht="11.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B19" s="43" t="s">
+      <c r="B19" s="51" t="s">
         <v>21</v>
       </c>
-      <c r="C19" s="44"/>
-      <c r="D19" s="45"/>
+      <c r="C19" s="52"/>
+      <c r="D19" s="53"/>
       <c r="E19" s="7">
         <f>SUM(E4:E18)</f>
         <v>32.380000000000003</v>
@@ -3008,13 +3008,13 @@
       <c r="F19" s="8"/>
     </row>
     <row r="20" spans="2:6" ht="11.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B20" s="46" t="s">
+      <c r="B20" s="54" t="s">
         <v>19</v>
       </c>
-      <c r="C20" s="47"/>
-      <c r="D20" s="48"/>
-      <c r="E20" s="49"/>
-      <c r="F20" s="50"/>
+      <c r="C20" s="55"/>
+      <c r="D20" s="56"/>
+      <c r="E20" s="57"/>
+      <c r="F20" s="58"/>
     </row>
     <row r="21" spans="2:6" ht="11.25" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="22" spans="2:6" ht="11.25" customHeight="1" x14ac:dyDescent="0.35">

</xml_diff>